<commit_message>
REALLY fix Palestine ISO3
</commit_message>
<xml_diff>
--- a/CountryReconciler/reconciler/files/country_list.xlsx
+++ b/CountryReconciler/reconciler/files/country_list.xlsx
@@ -7844,6 +7844,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12696825" cy="12849225"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8136,8 +8184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL176" workbookViewId="0">
-      <selection activeCell="AX185" sqref="AX185"/>
+    <sheetView tabSelected="1" topLeftCell="C151" workbookViewId="0">
+      <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -34311,7 +34359,7 @@
         <v>1607</v>
       </c>
       <c r="D185" s="38" t="s">
-        <v>1608</v>
+        <v>1612</v>
       </c>
       <c r="E185" s="3"/>
       <c r="F185" s="7" t="s">

</xml_diff>

<commit_message>
Recognize mroe faostat codes
</commit_message>
<xml_diff>
--- a/CountryReconciler/reconciler/files/country_list.xlsx
+++ b/CountryReconciler/reconciler/files/country_list.xlsx
@@ -7892,6 +7892,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12696825" cy="12849225"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8184,8 +8232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C151" workbookViewId="0">
-      <selection activeCell="F178" sqref="F178"/>
+    <sheetView tabSelected="1" topLeftCell="AQ74" workbookViewId="0">
+      <selection activeCell="AV103" sqref="AV103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21013,7 +21061,9 @@
       <c r="AU90" s="7">
         <v>-99</v>
       </c>
-      <c r="AV90" s="24"/>
+      <c r="AV90" s="24">
+        <v>85</v>
+      </c>
     </row>
     <row r="91" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
@@ -22652,7 +22702,9 @@
       <c r="AU102" s="7">
         <v>-99</v>
       </c>
-      <c r="AV102" s="24"/>
+      <c r="AV102" s="24">
+        <v>264</v>
+      </c>
     </row>
     <row r="103" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
@@ -29822,7 +29874,9 @@
       <c r="AU152" s="7">
         <v>-99</v>
       </c>
-      <c r="AV152" s="24"/>
+      <c r="AV152" s="24">
+        <v>163</v>
+      </c>
     </row>
     <row r="153" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
@@ -31326,7 +31380,9 @@
       <c r="AU163" s="7">
         <v>-99</v>
       </c>
-      <c r="AV163" s="24"/>
+      <c r="AV163" s="24">
+        <v>161</v>
+      </c>
     </row>
     <row r="164" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
@@ -33050,7 +33106,9 @@
       <c r="AU175" s="7">
         <v>-99</v>
       </c>
-      <c r="AV175" s="24"/>
+      <c r="AV175" s="24">
+        <v>172</v>
+      </c>
     </row>
     <row r="176" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
@@ -35414,7 +35472,9 @@
       <c r="AU192" s="7">
         <v>1</v>
       </c>
-      <c r="AV192" s="24"/>
+      <c r="AV192" s="24">
+        <v>205</v>
+      </c>
     </row>
     <row r="193" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
@@ -40652,6 +40712,9 @@
       <c r="AU229" s="17">
         <v>1</v>
       </c>
+      <c r="AV229">
+        <v>227</v>
+      </c>
     </row>
     <row r="230" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A230" s="17" t="s">
@@ -42231,7 +42294,9 @@
       <c r="AU240" s="7">
         <v>-99</v>
       </c>
-      <c r="AV240" s="24"/>
+      <c r="AV240" s="24">
+        <v>240</v>
+      </c>
     </row>
     <row r="241" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A241" s="17" t="s">

</xml_diff>